<commit_message>
Update people.xlsx with Lauren's info
</commit_message>
<xml_diff>
--- a/people.xlsx
+++ b/people.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c3f52bd1882c5245/sm_lab/projects/websites/chbv/chbv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="131" documentId="8_{EADF6017-5F87-0A4F-AF0D-7723D1C651F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F5C7F29-AC5E-A342-B7BD-D93DB05342C9}"/>
+  <xr:revisionPtr revIDLastSave="151" documentId="8_{EADF6017-5F87-0A4F-AF0D-7723D1C651F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F73D5F3-AFD1-9843-8032-19196AD9D663}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{3FDC604F-37A2-464A-9E1A-14A6423DCD4F}"/>
+    <workbookView xWindow="17920" yWindow="500" windowWidth="17920" windowHeight="20720" xr2:uid="{3FDC604F-37A2-464A-9E1A-14A6423DCD4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$34</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="177">
   <si>
     <t>email</t>
   </si>
@@ -558,6 +558,18 @@
   </si>
   <si>
     <t>Jim is a Principal Software Engineer at the Broad Institute and a McCarroll Lab member.  Jim develops new methods to analyze scRNASeq data and assists in workflow/QC design of scRNASeq datasets for large projects.  His previous work includes the development of the Drop-Seq software toolkit that processes data from raw reads to expression matrixes, as well as tools to demultiplex cellular villages (Dropulation) and infer donor proportions in low coverage DNA sequencing (Census).</t>
+  </si>
+  <si>
+    <t>Lauren</t>
+  </si>
+  <si>
+    <t>Macaisa</t>
+  </si>
+  <si>
+    <t>macaisa@broadinstitute.org</t>
+  </si>
+  <si>
+    <t>Lauren is a Research Associate II focused on organizing and optimizing wet lab protocols for the McCarroll &amp; Macosko BICAN lab efforts. Prior to working at the Broad, Lauren worked at Moffitt Cancer Center developing immunotherapy treatments for breast cancer. She graduated from University of North Florida with her B.S. in Behavioral Neuroscience and is pursuing her M.S. in Biotechnology from Northeastern.</t>
   </si>
 </sst>
 </file>
@@ -637,6 +649,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -936,10 +952,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{913DB89F-B24C-9A40-89FD-2CA7843C4F41}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection sqref="A1:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1481,48 +1497,42 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>150</v>
+        <v>173</v>
       </c>
       <c r="B23" t="s">
-        <v>151</v>
+        <v>174</v>
       </c>
       <c r="C23">
         <v>5</v>
       </c>
-      <c r="E23" t="s">
-        <v>54</v>
-      </c>
       <c r="F23" t="s">
-        <v>86</v>
+        <v>175</v>
       </c>
       <c r="G23" t="s">
-        <v>55</v>
+        <v>176</v>
       </c>
       <c r="H23" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>152</v>
+      <c r="A24" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="B24" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C24">
         <v>6</v>
       </c>
-      <c r="D24" t="s">
-        <v>100</v>
-      </c>
       <c r="E24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G24" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H24" t="s">
         <v>45</v>
@@ -1530,22 +1540,25 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B25" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C25">
         <v>7</v>
       </c>
+      <c r="D25" t="s">
+        <v>100</v>
+      </c>
       <c r="E25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H25" t="s">
         <v>45</v>
@@ -1553,22 +1566,22 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B26" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C26">
         <v>8</v>
       </c>
       <c r="E26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G26" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H26" t="s">
         <v>45</v>
@@ -1576,25 +1589,22 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B27" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C27">
         <v>9</v>
       </c>
-      <c r="D27" t="s">
-        <v>97</v>
-      </c>
       <c r="E27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G27" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H27" t="s">
         <v>45</v>
@@ -1602,48 +1612,51 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>114</v>
+        <v>158</v>
       </c>
       <c r="B28" t="s">
-        <v>115</v>
+        <v>159</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E28" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="F28" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="G28" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="H28" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B29" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>98</v>
       </c>
       <c r="E29" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G29" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H29" t="s">
         <v>26</v>
@@ -1651,22 +1664,22 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B30" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G30" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H30" t="s">
         <v>26</v>
@@ -1674,22 +1687,22 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B31" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C31">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E31" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G31" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H31" t="s">
         <v>26</v>
@@ -1697,22 +1710,22 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B32" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C32">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E32" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G32" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H32" t="s">
         <v>26</v>
@@ -1720,34 +1733,57 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B33" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C33">
-        <v>6</v>
-      </c>
-      <c r="D33" t="s">
-        <v>99</v>
+        <v>5</v>
       </c>
       <c r="E33" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G33" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H33" t="s">
         <v>26</v>
       </c>
     </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>124</v>
+      </c>
+      <c r="B34" t="s">
+        <v>125</v>
+      </c>
+      <c r="C34">
+        <v>6</v>
+      </c>
+      <c r="D34" t="s">
+        <v>99</v>
+      </c>
+      <c r="E34" t="s">
+        <v>24</v>
+      </c>
+      <c r="F34" t="s">
+        <v>73</v>
+      </c>
+      <c r="G34" t="s">
+        <v>25</v>
+      </c>
+      <c r="H34" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H32" xr:uid="{913DB89F-B24C-9A40-89FD-2CA7843C4F41}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H33">
-      <sortCondition ref="H1:H33"/>
+  <autoFilter ref="A1:H34" xr:uid="{913DB89F-B24C-9A40-89FD-2CA7843C4F41}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H34">
+      <sortCondition ref="H1:H34"/>
     </sortState>
   </autoFilter>
   <hyperlinks>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ broadinstitute/chbv@bf4b579c5e3ae61510fefcaca64aa87da1fe3ee1 🚀
</commit_message>
<xml_diff>
--- a/people.xlsx
+++ b/people.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c3f52bd1882c5245/sm_lab/projects/websites/chbv/chbv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="131" documentId="8_{EADF6017-5F87-0A4F-AF0D-7723D1C651F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F5C7F29-AC5E-A342-B7BD-D93DB05342C9}"/>
+  <xr:revisionPtr revIDLastSave="151" documentId="8_{EADF6017-5F87-0A4F-AF0D-7723D1C651F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F73D5F3-AFD1-9843-8032-19196AD9D663}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{3FDC604F-37A2-464A-9E1A-14A6423DCD4F}"/>
+    <workbookView xWindow="17920" yWindow="500" windowWidth="17920" windowHeight="20720" xr2:uid="{3FDC604F-37A2-464A-9E1A-14A6423DCD4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$34</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="177">
   <si>
     <t>email</t>
   </si>
@@ -558,6 +558,18 @@
   </si>
   <si>
     <t>Jim is a Principal Software Engineer at the Broad Institute and a McCarroll Lab member.  Jim develops new methods to analyze scRNASeq data and assists in workflow/QC design of scRNASeq datasets for large projects.  His previous work includes the development of the Drop-Seq software toolkit that processes data from raw reads to expression matrixes, as well as tools to demultiplex cellular villages (Dropulation) and infer donor proportions in low coverage DNA sequencing (Census).</t>
+  </si>
+  <si>
+    <t>Lauren</t>
+  </si>
+  <si>
+    <t>Macaisa</t>
+  </si>
+  <si>
+    <t>macaisa@broadinstitute.org</t>
+  </si>
+  <si>
+    <t>Lauren is a Research Associate II focused on organizing and optimizing wet lab protocols for the McCarroll &amp; Macosko BICAN lab efforts. Prior to working at the Broad, Lauren worked at Moffitt Cancer Center developing immunotherapy treatments for breast cancer. She graduated from University of North Florida with her B.S. in Behavioral Neuroscience and is pursuing her M.S. in Biotechnology from Northeastern.</t>
   </si>
 </sst>
 </file>
@@ -637,6 +649,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -936,10 +952,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{913DB89F-B24C-9A40-89FD-2CA7843C4F41}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection sqref="A1:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1481,48 +1497,42 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>150</v>
+        <v>173</v>
       </c>
       <c r="B23" t="s">
-        <v>151</v>
+        <v>174</v>
       </c>
       <c r="C23">
         <v>5</v>
       </c>
-      <c r="E23" t="s">
-        <v>54</v>
-      </c>
       <c r="F23" t="s">
-        <v>86</v>
+        <v>175</v>
       </c>
       <c r="G23" t="s">
-        <v>55</v>
+        <v>176</v>
       </c>
       <c r="H23" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>152</v>
+      <c r="A24" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="B24" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C24">
         <v>6</v>
       </c>
-      <c r="D24" t="s">
-        <v>100</v>
-      </c>
       <c r="E24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G24" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H24" t="s">
         <v>45</v>
@@ -1530,22 +1540,25 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B25" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C25">
         <v>7</v>
       </c>
+      <c r="D25" t="s">
+        <v>100</v>
+      </c>
       <c r="E25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H25" t="s">
         <v>45</v>
@@ -1553,22 +1566,22 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B26" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C26">
         <v>8</v>
       </c>
       <c r="E26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G26" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H26" t="s">
         <v>45</v>
@@ -1576,25 +1589,22 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B27" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C27">
         <v>9</v>
       </c>
-      <c r="D27" t="s">
-        <v>97</v>
-      </c>
       <c r="E27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G27" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H27" t="s">
         <v>45</v>
@@ -1602,48 +1612,51 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>114</v>
+        <v>158</v>
       </c>
       <c r="B28" t="s">
-        <v>115</v>
+        <v>159</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E28" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="F28" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="G28" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="H28" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B29" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>98</v>
       </c>
       <c r="E29" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G29" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H29" t="s">
         <v>26</v>
@@ -1651,22 +1664,22 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B30" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G30" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H30" t="s">
         <v>26</v>
@@ -1674,22 +1687,22 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B31" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C31">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E31" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G31" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H31" t="s">
         <v>26</v>
@@ -1697,22 +1710,22 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B32" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C32">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E32" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G32" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H32" t="s">
         <v>26</v>
@@ -1720,34 +1733,57 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B33" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C33">
-        <v>6</v>
-      </c>
-      <c r="D33" t="s">
-        <v>99</v>
+        <v>5</v>
       </c>
       <c r="E33" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G33" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H33" t="s">
         <v>26</v>
       </c>
     </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>124</v>
+      </c>
+      <c r="B34" t="s">
+        <v>125</v>
+      </c>
+      <c r="C34">
+        <v>6</v>
+      </c>
+      <c r="D34" t="s">
+        <v>99</v>
+      </c>
+      <c r="E34" t="s">
+        <v>24</v>
+      </c>
+      <c r="F34" t="s">
+        <v>73</v>
+      </c>
+      <c r="G34" t="s">
+        <v>25</v>
+      </c>
+      <c r="H34" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H32" xr:uid="{913DB89F-B24C-9A40-89FD-2CA7843C4F41}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H33">
-      <sortCondition ref="H1:H33"/>
+  <autoFilter ref="A1:H34" xr:uid="{913DB89F-B24C-9A40-89FD-2CA7843C4F41}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H34">
+      <sortCondition ref="H1:H34"/>
     </sortState>
   </autoFilter>
   <hyperlinks>

</xml_diff>

<commit_message>
Add Haley Fritch to teams page
</commit_message>
<xml_diff>
--- a/people.xlsx
+++ b/people.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c3f52bd1882c5245/sm_lab/projects/websites/chbv/chbv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="151" documentId="8_{EADF6017-5F87-0A4F-AF0D-7723D1C651F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F73D5F3-AFD1-9843-8032-19196AD9D663}"/>
+  <xr:revisionPtr revIDLastSave="176" documentId="8_{EADF6017-5F87-0A4F-AF0D-7723D1C651F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC86238B-9958-274B-ADFB-F40AE4405F65}"/>
   <bookViews>
-    <workbookView xWindow="17920" yWindow="500" windowWidth="17920" windowHeight="20720" xr2:uid="{3FDC604F-37A2-464A-9E1A-14A6423DCD4F}"/>
+    <workbookView xWindow="1140" yWindow="500" windowWidth="34700" windowHeight="20720" xr2:uid="{3FDC604F-37A2-464A-9E1A-14A6423DCD4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$34</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="181">
   <si>
     <t>email</t>
   </si>
@@ -570,6 +571,18 @@
   </si>
   <si>
     <t>Lauren is a Research Associate II focused on organizing and optimizing wet lab protocols for the McCarroll &amp; Macosko BICAN lab efforts. Prior to working at the Broad, Lauren worked at Moffitt Cancer Center developing immunotherapy treatments for breast cancer. She graduated from University of North Florida with her B.S. in Behavioral Neuroscience and is pursuing her M.S. in Biotechnology from Northeastern.</t>
+  </si>
+  <si>
+    <t>fritch@broadinstitute.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haley joined the McCarroll Lab as a computational scientist in May 2023. She received a PhD in cognitive neuroscience from Boston College and a BS in psychobiology from UCLA. Prior to joining the lab, Haley used machine learning methods to analyze neuroimaging data and gained experience with natural language processing. </t>
+  </si>
+  <si>
+    <t>Haley</t>
+  </si>
+  <si>
+    <t>Fritch</t>
   </si>
 </sst>
 </file>
@@ -952,19 +965,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{913DB89F-B24C-9A40-89FD-2CA7843C4F41}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H23"/>
+      <selection activeCell="C7" sqref="C7:C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="25.1640625" customWidth="1"/>
-    <col min="6" max="6" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
@@ -1150,10 +1157,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="B8" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -1161,11 +1168,11 @@
       <c r="D8" t="s">
         <v>97</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>95</v>
+      <c r="F8" t="s">
+        <v>177</v>
       </c>
       <c r="G8" t="s">
-        <v>96</v>
+        <v>178</v>
       </c>
       <c r="H8" t="s">
         <v>28</v>
@@ -1173,10 +1180,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>128</v>
+        <v>166</v>
       </c>
       <c r="B9" t="s">
-        <v>129</v>
+        <v>167</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -1184,14 +1191,11 @@
       <c r="D9" t="s">
         <v>97</v>
       </c>
-      <c r="E9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" t="s">
-        <v>75</v>
+      <c r="F9" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="G9" t="s">
-        <v>32</v>
+        <v>96</v>
       </c>
       <c r="H9" t="s">
         <v>28</v>
@@ -1199,17 +1203,25 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>162</v>
+        <v>128</v>
       </c>
       <c r="B10" t="s">
-        <v>163</v>
+        <v>129</v>
       </c>
       <c r="C10">
         <v>4</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="D10" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" t="s">
+        <v>75</v>
+      </c>
       <c r="G10" t="s">
-        <v>171</v>
+        <v>32</v>
       </c>
       <c r="H10" t="s">
         <v>28</v>
@@ -1217,63 +1229,61 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>130</v>
+        <v>162</v>
       </c>
       <c r="B11" t="s">
-        <v>131</v>
+        <v>163</v>
       </c>
       <c r="C11">
         <v>5</v>
       </c>
-      <c r="E11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" t="s">
-        <v>76</v>
-      </c>
+      <c r="F11" s="1"/>
       <c r="G11" t="s">
-        <v>34</v>
+        <v>171</v>
       </c>
       <c r="H11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>161</v>
+      <c r="A12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12" t="s">
+        <v>131</v>
       </c>
       <c r="C12">
         <v>6</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="F12" s="1" t="s">
-        <v>92</v>
+      <c r="E12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" t="s">
+        <v>76</v>
       </c>
       <c r="G12" t="s">
-        <v>93</v>
+        <v>34</v>
       </c>
       <c r="H12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>164</v>
-      </c>
-      <c r="B13" t="s">
-        <v>165</v>
+      <c r="A13" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>161</v>
       </c>
       <c r="C13">
         <v>7</v>
       </c>
+      <c r="D13" s="2"/>
       <c r="F13" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G13" t="s">
-        <v>172</v>
+        <v>93</v>
       </c>
       <c r="H13" t="s">
         <v>28</v>
@@ -1281,25 +1291,19 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>132</v>
+        <v>164</v>
       </c>
       <c r="B14" t="s">
-        <v>133</v>
+        <v>165</v>
       </c>
       <c r="C14">
         <v>8</v>
       </c>
-      <c r="D14" t="s">
-        <v>97</v>
-      </c>
-      <c r="E14" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" t="s">
-        <v>77</v>
+      <c r="F14" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="G14" t="s">
-        <v>36</v>
+        <v>172</v>
       </c>
       <c r="H14" t="s">
         <v>28</v>
@@ -1307,22 +1311,25 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C15">
         <v>9</v>
       </c>
+      <c r="D15" t="s">
+        <v>97</v>
+      </c>
       <c r="E15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H15" t="s">
         <v>28</v>
@@ -1330,22 +1337,22 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B16" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C16">
         <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H16" t="s">
         <v>28</v>
@@ -1353,25 +1360,22 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B17" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C17">
         <v>11</v>
       </c>
-      <c r="D17" t="s">
-        <v>99</v>
-      </c>
       <c r="E17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H17" t="s">
         <v>28</v>
@@ -1379,22 +1383,25 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B18" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C18">
         <v>12</v>
       </c>
+      <c r="D18" t="s">
+        <v>99</v>
+      </c>
       <c r="E18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H18" t="s">
         <v>28</v>
@@ -1402,45 +1409,45 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B19" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E19" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G19" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H19" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B20" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H20" t="s">
         <v>45</v>
@@ -1448,25 +1455,22 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C21">
-        <v>3</v>
-      </c>
-      <c r="D21" t="s">
-        <v>97</v>
+        <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H21" t="s">
         <v>45</v>
@@ -1474,22 +1478,25 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B22" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>97</v>
       </c>
       <c r="E22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H22" t="s">
         <v>45</v>
@@ -1497,68 +1504,65 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
       <c r="B23" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
       <c r="C23">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="E23" t="s">
+        <v>52</v>
       </c>
       <c r="F23" t="s">
-        <v>175</v>
+        <v>85</v>
       </c>
       <c r="G23" t="s">
-        <v>176</v>
+        <v>53</v>
       </c>
       <c r="H23" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>150</v>
+      <c r="A24" t="s">
+        <v>173</v>
       </c>
       <c r="B24" t="s">
-        <v>151</v>
+        <v>174</v>
       </c>
       <c r="C24">
-        <v>6</v>
-      </c>
-      <c r="E24" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="F24" t="s">
-        <v>86</v>
+        <v>175</v>
       </c>
       <c r="G24" t="s">
-        <v>55</v>
+        <v>176</v>
       </c>
       <c r="H24" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>152</v>
+      <c r="A25" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="B25" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C25">
-        <v>7</v>
-      </c>
-      <c r="D25" t="s">
-        <v>100</v>
+        <v>6</v>
       </c>
       <c r="E25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H25" t="s">
         <v>45</v>
@@ -1566,22 +1570,25 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B26" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C26">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="D26" t="s">
+        <v>100</v>
       </c>
       <c r="E26" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G26" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H26" t="s">
         <v>45</v>
@@ -1589,22 +1596,22 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B27" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C27">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E27" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H27" t="s">
         <v>45</v>
@@ -1612,25 +1619,22 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B28" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C28">
-        <v>10</v>
-      </c>
-      <c r="D28" t="s">
-        <v>97</v>
+        <v>9</v>
       </c>
       <c r="E28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G28" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H28" t="s">
         <v>45</v>
@@ -1638,48 +1642,51 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>114</v>
+        <v>158</v>
       </c>
       <c r="B29" t="s">
-        <v>115</v>
+        <v>159</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E29" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="F29" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="G29" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="H29" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B30" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C30">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>98</v>
       </c>
       <c r="E30" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G30" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H30" t="s">
         <v>26</v>
@@ -1687,22 +1694,22 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B31" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E31" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G31" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H31" t="s">
         <v>26</v>
@@ -1710,22 +1717,22 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B32" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C32">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E32" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G32" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H32" t="s">
         <v>26</v>
@@ -1733,22 +1740,22 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B33" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C33">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E33" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G33" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H33" t="s">
         <v>26</v>
@@ -1756,42 +1763,129 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C34">
-        <v>6</v>
-      </c>
-      <c r="D34" t="s">
-        <v>99</v>
+        <v>5</v>
       </c>
       <c r="E34" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G34" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H34" t="s">
         <v>26</v>
       </c>
     </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>124</v>
+      </c>
+      <c r="B35" t="s">
+        <v>125</v>
+      </c>
+      <c r="C35">
+        <v>6</v>
+      </c>
+      <c r="D35" t="s">
+        <v>99</v>
+      </c>
+      <c r="E35" t="s">
+        <v>24</v>
+      </c>
+      <c r="F35" t="s">
+        <v>73</v>
+      </c>
+      <c r="G35" t="s">
+        <v>25</v>
+      </c>
+      <c r="H35" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H34" xr:uid="{913DB89F-B24C-9A40-89FD-2CA7843C4F41}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H34">
-      <sortCondition ref="H1:H34"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H35">
+      <sortCondition ref="H1:H35"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
     <hyperlink ref="F6" r:id="rId1" xr:uid="{EF70C838-9454-A340-875B-3D4829496F9E}"/>
-    <hyperlink ref="F12" r:id="rId2" xr:uid="{5DEF1B66-0C25-744A-8D21-CF21443745D2}"/>
-    <hyperlink ref="F13" r:id="rId3" xr:uid="{05B46BA3-D647-FD42-AB3D-3CEEFA5D5FF1}"/>
-    <hyperlink ref="F8" r:id="rId4" xr:uid="{24BE637A-2716-3B49-A1E8-71436F3E485C}"/>
+    <hyperlink ref="F13" r:id="rId2" xr:uid="{5DEF1B66-0C25-744A-8D21-CF21443745D2}"/>
+    <hyperlink ref="F14" r:id="rId3" xr:uid="{05B46BA3-D647-FD42-AB3D-3CEEFA5D5FF1}"/>
+    <hyperlink ref="F9" r:id="rId4" xr:uid="{24BE637A-2716-3B49-A1E8-71436F3E485C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C47BFFC-A8EF-3F42-B9D9-B405CCCF7827}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G2" t="s">
+        <v>178</v>
+      </c>
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Deploying to gh-pages from @ broadinstitute/chbv@088c1ac4577efc635a1f34f94b4440cf23980b5f 🚀
</commit_message>
<xml_diff>
--- a/people.xlsx
+++ b/people.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c3f52bd1882c5245/sm_lab/projects/websites/chbv/chbv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="151" documentId="8_{EADF6017-5F87-0A4F-AF0D-7723D1C651F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F73D5F3-AFD1-9843-8032-19196AD9D663}"/>
+  <xr:revisionPtr revIDLastSave="176" documentId="8_{EADF6017-5F87-0A4F-AF0D-7723D1C651F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC86238B-9958-274B-ADFB-F40AE4405F65}"/>
   <bookViews>
-    <workbookView xWindow="17920" yWindow="500" windowWidth="17920" windowHeight="20720" xr2:uid="{3FDC604F-37A2-464A-9E1A-14A6423DCD4F}"/>
+    <workbookView xWindow="1140" yWindow="500" windowWidth="34700" windowHeight="20720" xr2:uid="{3FDC604F-37A2-464A-9E1A-14A6423DCD4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$34</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="181">
   <si>
     <t>email</t>
   </si>
@@ -570,6 +571,18 @@
   </si>
   <si>
     <t>Lauren is a Research Associate II focused on organizing and optimizing wet lab protocols for the McCarroll &amp; Macosko BICAN lab efforts. Prior to working at the Broad, Lauren worked at Moffitt Cancer Center developing immunotherapy treatments for breast cancer. She graduated from University of North Florida with her B.S. in Behavioral Neuroscience and is pursuing her M.S. in Biotechnology from Northeastern.</t>
+  </si>
+  <si>
+    <t>fritch@broadinstitute.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haley joined the McCarroll Lab as a computational scientist in May 2023. She received a PhD in cognitive neuroscience from Boston College and a BS in psychobiology from UCLA. Prior to joining the lab, Haley used machine learning methods to analyze neuroimaging data and gained experience with natural language processing. </t>
+  </si>
+  <si>
+    <t>Haley</t>
+  </si>
+  <si>
+    <t>Fritch</t>
   </si>
 </sst>
 </file>
@@ -952,19 +965,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{913DB89F-B24C-9A40-89FD-2CA7843C4F41}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H23"/>
+      <selection activeCell="C7" sqref="C7:C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="25.1640625" customWidth="1"/>
-    <col min="6" max="6" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
@@ -1150,10 +1157,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="B8" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -1161,11 +1168,11 @@
       <c r="D8" t="s">
         <v>97</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>95</v>
+      <c r="F8" t="s">
+        <v>177</v>
       </c>
       <c r="G8" t="s">
-        <v>96</v>
+        <v>178</v>
       </c>
       <c r="H8" t="s">
         <v>28</v>
@@ -1173,10 +1180,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>128</v>
+        <v>166</v>
       </c>
       <c r="B9" t="s">
-        <v>129</v>
+        <v>167</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -1184,14 +1191,11 @@
       <c r="D9" t="s">
         <v>97</v>
       </c>
-      <c r="E9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" t="s">
-        <v>75</v>
+      <c r="F9" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="G9" t="s">
-        <v>32</v>
+        <v>96</v>
       </c>
       <c r="H9" t="s">
         <v>28</v>
@@ -1199,17 +1203,25 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>162</v>
+        <v>128</v>
       </c>
       <c r="B10" t="s">
-        <v>163</v>
+        <v>129</v>
       </c>
       <c r="C10">
         <v>4</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="D10" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" t="s">
+        <v>75</v>
+      </c>
       <c r="G10" t="s">
-        <v>171</v>
+        <v>32</v>
       </c>
       <c r="H10" t="s">
         <v>28</v>
@@ -1217,63 +1229,61 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>130</v>
+        <v>162</v>
       </c>
       <c r="B11" t="s">
-        <v>131</v>
+        <v>163</v>
       </c>
       <c r="C11">
         <v>5</v>
       </c>
-      <c r="E11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" t="s">
-        <v>76</v>
-      </c>
+      <c r="F11" s="1"/>
       <c r="G11" t="s">
-        <v>34</v>
+        <v>171</v>
       </c>
       <c r="H11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>161</v>
+      <c r="A12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12" t="s">
+        <v>131</v>
       </c>
       <c r="C12">
         <v>6</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="F12" s="1" t="s">
-        <v>92</v>
+      <c r="E12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" t="s">
+        <v>76</v>
       </c>
       <c r="G12" t="s">
-        <v>93</v>
+        <v>34</v>
       </c>
       <c r="H12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>164</v>
-      </c>
-      <c r="B13" t="s">
-        <v>165</v>
+      <c r="A13" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>161</v>
       </c>
       <c r="C13">
         <v>7</v>
       </c>
+      <c r="D13" s="2"/>
       <c r="F13" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G13" t="s">
-        <v>172</v>
+        <v>93</v>
       </c>
       <c r="H13" t="s">
         <v>28</v>
@@ -1281,25 +1291,19 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>132</v>
+        <v>164</v>
       </c>
       <c r="B14" t="s">
-        <v>133</v>
+        <v>165</v>
       </c>
       <c r="C14">
         <v>8</v>
       </c>
-      <c r="D14" t="s">
-        <v>97</v>
-      </c>
-      <c r="E14" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" t="s">
-        <v>77</v>
+      <c r="F14" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="G14" t="s">
-        <v>36</v>
+        <v>172</v>
       </c>
       <c r="H14" t="s">
         <v>28</v>
@@ -1307,22 +1311,25 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C15">
         <v>9</v>
       </c>
+      <c r="D15" t="s">
+        <v>97</v>
+      </c>
       <c r="E15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H15" t="s">
         <v>28</v>
@@ -1330,22 +1337,22 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B16" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C16">
         <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H16" t="s">
         <v>28</v>
@@ -1353,25 +1360,22 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B17" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C17">
         <v>11</v>
       </c>
-      <c r="D17" t="s">
-        <v>99</v>
-      </c>
       <c r="E17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H17" t="s">
         <v>28</v>
@@ -1379,22 +1383,25 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B18" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C18">
         <v>12</v>
       </c>
+      <c r="D18" t="s">
+        <v>99</v>
+      </c>
       <c r="E18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H18" t="s">
         <v>28</v>
@@ -1402,45 +1409,45 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B19" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E19" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G19" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H19" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B20" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H20" t="s">
         <v>45</v>
@@ -1448,25 +1455,22 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C21">
-        <v>3</v>
-      </c>
-      <c r="D21" t="s">
-        <v>97</v>
+        <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H21" t="s">
         <v>45</v>
@@ -1474,22 +1478,25 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B22" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>97</v>
       </c>
       <c r="E22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H22" t="s">
         <v>45</v>
@@ -1497,68 +1504,65 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
       <c r="B23" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
       <c r="C23">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="E23" t="s">
+        <v>52</v>
       </c>
       <c r="F23" t="s">
-        <v>175</v>
+        <v>85</v>
       </c>
       <c r="G23" t="s">
-        <v>176</v>
+        <v>53</v>
       </c>
       <c r="H23" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>150</v>
+      <c r="A24" t="s">
+        <v>173</v>
       </c>
       <c r="B24" t="s">
-        <v>151</v>
+        <v>174</v>
       </c>
       <c r="C24">
-        <v>6</v>
-      </c>
-      <c r="E24" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="F24" t="s">
-        <v>86</v>
+        <v>175</v>
       </c>
       <c r="G24" t="s">
-        <v>55</v>
+        <v>176</v>
       </c>
       <c r="H24" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>152</v>
+      <c r="A25" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="B25" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C25">
-        <v>7</v>
-      </c>
-      <c r="D25" t="s">
-        <v>100</v>
+        <v>6</v>
       </c>
       <c r="E25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H25" t="s">
         <v>45</v>
@@ -1566,22 +1570,25 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B26" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C26">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="D26" t="s">
+        <v>100</v>
       </c>
       <c r="E26" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G26" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H26" t="s">
         <v>45</v>
@@ -1589,22 +1596,22 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B27" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C27">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E27" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H27" t="s">
         <v>45</v>
@@ -1612,25 +1619,22 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B28" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C28">
-        <v>10</v>
-      </c>
-      <c r="D28" t="s">
-        <v>97</v>
+        <v>9</v>
       </c>
       <c r="E28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G28" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H28" t="s">
         <v>45</v>
@@ -1638,48 +1642,51 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>114</v>
+        <v>158</v>
       </c>
       <c r="B29" t="s">
-        <v>115</v>
+        <v>159</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E29" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="F29" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="G29" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="H29" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B30" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C30">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>98</v>
       </c>
       <c r="E30" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G30" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H30" t="s">
         <v>26</v>
@@ -1687,22 +1694,22 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B31" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E31" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G31" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H31" t="s">
         <v>26</v>
@@ -1710,22 +1717,22 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B32" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C32">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E32" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G32" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H32" t="s">
         <v>26</v>
@@ -1733,22 +1740,22 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B33" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C33">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E33" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G33" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H33" t="s">
         <v>26</v>
@@ -1756,42 +1763,129 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C34">
-        <v>6</v>
-      </c>
-      <c r="D34" t="s">
-        <v>99</v>
+        <v>5</v>
       </c>
       <c r="E34" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G34" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H34" t="s">
         <v>26</v>
       </c>
     </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>124</v>
+      </c>
+      <c r="B35" t="s">
+        <v>125</v>
+      </c>
+      <c r="C35">
+        <v>6</v>
+      </c>
+      <c r="D35" t="s">
+        <v>99</v>
+      </c>
+      <c r="E35" t="s">
+        <v>24</v>
+      </c>
+      <c r="F35" t="s">
+        <v>73</v>
+      </c>
+      <c r="G35" t="s">
+        <v>25</v>
+      </c>
+      <c r="H35" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H34" xr:uid="{913DB89F-B24C-9A40-89FD-2CA7843C4F41}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H34">
-      <sortCondition ref="H1:H34"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H35">
+      <sortCondition ref="H1:H35"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
     <hyperlink ref="F6" r:id="rId1" xr:uid="{EF70C838-9454-A340-875B-3D4829496F9E}"/>
-    <hyperlink ref="F12" r:id="rId2" xr:uid="{5DEF1B66-0C25-744A-8D21-CF21443745D2}"/>
-    <hyperlink ref="F13" r:id="rId3" xr:uid="{05B46BA3-D647-FD42-AB3D-3CEEFA5D5FF1}"/>
-    <hyperlink ref="F8" r:id="rId4" xr:uid="{24BE637A-2716-3B49-A1E8-71436F3E485C}"/>
+    <hyperlink ref="F13" r:id="rId2" xr:uid="{5DEF1B66-0C25-744A-8D21-CF21443745D2}"/>
+    <hyperlink ref="F14" r:id="rId3" xr:uid="{05B46BA3-D647-FD42-AB3D-3CEEFA5D5FF1}"/>
+    <hyperlink ref="F9" r:id="rId4" xr:uid="{24BE637A-2716-3B49-A1E8-71436F3E485C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C47BFFC-A8EF-3F42-B9D9-B405CCCF7827}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G2" t="s">
+        <v>178</v>
+      </c>
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix issue #11: add new member kathleen to website
</commit_message>
<xml_diff>
--- a/people.xlsx
+++ b/people.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c3f52bd1882c5245/sm_lab/projects/websites/chbv/chbv/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nrockwei/Library/CloudStorage/OneDrive-Personal/sm_lab/projects/websites/chbv/chbv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="176" documentId="8_{EADF6017-5F87-0A4F-AF0D-7723D1C651F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC86238B-9958-274B-ADFB-F40AE4405F65}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946DABF0-E1AB-CC46-8D1A-EF3775259AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="500" windowWidth="34700" windowHeight="20720" xr2:uid="{3FDC604F-37A2-464A-9E1A-14A6423DCD4F}"/>
+    <workbookView xWindow="1140" yWindow="500" windowWidth="34700" windowHeight="20720" activeTab="1" xr2:uid="{3FDC604F-37A2-464A-9E1A-14A6423DCD4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="185">
   <si>
     <t>email</t>
   </si>
@@ -583,6 +583,18 @@
   </si>
   <si>
     <t>Fritch</t>
+  </si>
+  <si>
+    <t>Sadie</t>
+  </si>
+  <si>
+    <t>Drouin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sadie is a Research Associate I for the McCarroll &amp; Macosko BICAN project. She is a recent graduate from Wheaton College MA with a B.S. in Neuroscience on the Pre-Medical Track. Prior to joining the BICAN project, in her Behavioral Neuroscience lab she completed a senior honors thesis titled: The effects of maternal separation and social isolation on memory and myelin in adolescent rats. In addition to being a research associate, she is also a medical assistant in primary care and sports medicine at DMC primary care. </t>
+  </si>
+  <si>
+    <t>drouin@broadinstitute.org</t>
   </si>
 </sst>
 </file>
@@ -662,10 +674,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -965,10 +973,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{913DB89F-B24C-9A40-89FD-2CA7843C4F41}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1808,6 +1816,23 @@
       </c>
       <c r="H35" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>181</v>
+      </c>
+      <c r="B36" t="s">
+        <v>182</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="G36" t="s">
+        <v>183</v>
+      </c>
+      <c r="H36" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1821,6 +1846,7 @@
     <hyperlink ref="F13" r:id="rId2" xr:uid="{5DEF1B66-0C25-744A-8D21-CF21443745D2}"/>
     <hyperlink ref="F14" r:id="rId3" xr:uid="{05B46BA3-D647-FD42-AB3D-3CEEFA5D5FF1}"/>
     <hyperlink ref="F9" r:id="rId4" xr:uid="{24BE637A-2716-3B49-A1E8-71436F3E485C}"/>
+    <hyperlink ref="F36" r:id="rId5" xr:uid="{06EDA934-8DE4-0A41-88B2-4E0BE023A029}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1830,7 +1856,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C47BFFC-A8EF-3F42-B9D9-B405CCCF7827}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
@@ -1864,28 +1890,25 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F2" t="s">
-        <v>177</v>
+        <v>182</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>184</v>
       </c>
       <c r="G2" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="H2" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{6760BC2D-FC9E-B14B-A80F-A06DBA6C649E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Deploying to gh-pages from @ broadinstitute/chbv@a7e39f31d0e73c8eec725588f665bbe8431383b9 🚀
</commit_message>
<xml_diff>
--- a/people.xlsx
+++ b/people.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c3f52bd1882c5245/sm_lab/projects/websites/chbv/chbv/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nrockwei/Library/CloudStorage/OneDrive-Personal/sm_lab/projects/websites/chbv/chbv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="176" documentId="8_{EADF6017-5F87-0A4F-AF0D-7723D1C651F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC86238B-9958-274B-ADFB-F40AE4405F65}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946DABF0-E1AB-CC46-8D1A-EF3775259AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="500" windowWidth="34700" windowHeight="20720" xr2:uid="{3FDC604F-37A2-464A-9E1A-14A6423DCD4F}"/>
+    <workbookView xWindow="1140" yWindow="500" windowWidth="34700" windowHeight="20720" activeTab="1" xr2:uid="{3FDC604F-37A2-464A-9E1A-14A6423DCD4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="185">
   <si>
     <t>email</t>
   </si>
@@ -583,6 +583,18 @@
   </si>
   <si>
     <t>Fritch</t>
+  </si>
+  <si>
+    <t>Sadie</t>
+  </si>
+  <si>
+    <t>Drouin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sadie is a Research Associate I for the McCarroll &amp; Macosko BICAN project. She is a recent graduate from Wheaton College MA with a B.S. in Neuroscience on the Pre-Medical Track. Prior to joining the BICAN project, in her Behavioral Neuroscience lab she completed a senior honors thesis titled: The effects of maternal separation and social isolation on memory and myelin in adolescent rats. In addition to being a research associate, she is also a medical assistant in primary care and sports medicine at DMC primary care. </t>
+  </si>
+  <si>
+    <t>drouin@broadinstitute.org</t>
   </si>
 </sst>
 </file>
@@ -662,10 +674,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -965,10 +973,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{913DB89F-B24C-9A40-89FD-2CA7843C4F41}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1808,6 +1816,23 @@
       </c>
       <c r="H35" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>181</v>
+      </c>
+      <c r="B36" t="s">
+        <v>182</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="G36" t="s">
+        <v>183</v>
+      </c>
+      <c r="H36" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1821,6 +1846,7 @@
     <hyperlink ref="F13" r:id="rId2" xr:uid="{5DEF1B66-0C25-744A-8D21-CF21443745D2}"/>
     <hyperlink ref="F14" r:id="rId3" xr:uid="{05B46BA3-D647-FD42-AB3D-3CEEFA5D5FF1}"/>
     <hyperlink ref="F9" r:id="rId4" xr:uid="{24BE637A-2716-3B49-A1E8-71436F3E485C}"/>
+    <hyperlink ref="F36" r:id="rId5" xr:uid="{06EDA934-8DE4-0A41-88B2-4E0BE023A029}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1830,7 +1856,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C47BFFC-A8EF-3F42-B9D9-B405CCCF7827}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
@@ -1864,28 +1890,25 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F2" t="s">
-        <v>177</v>
+        <v>182</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>184</v>
       </c>
       <c r="G2" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="H2" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{6760BC2D-FC9E-B14B-A80F-A06DBA6C649E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add latest members and remove old members
 - Added the following:
    - Jonah Langlieb
    - Emily Finn
    - Mukund Raj
    - Jonah Silverman
    - Valerie Foley

 - Remove the following:
    - Jasmin Patel
    - Jonah Levin
    - Andrea Jiang
    - Vahid Gazestani
    - Nina Sachdev
</commit_message>
<xml_diff>
--- a/people.xlsx
+++ b/people.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nrockwei/Library/CloudStorage/OneDrive-Personal/sm_lab/projects/websites/chbv/chbv/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c3f52bd1882c5245/sm_lab/projects/websites/chbv/chbv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946DABF0-E1AB-CC46-8D1A-EF3775259AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="219" documentId="8_{EADF6017-5F87-0A4F-AF0D-7723D1C651F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{149D7C51-487F-934C-B96E-F05B3E4FC7A1}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="500" windowWidth="34700" windowHeight="20720" activeTab="1" xr2:uid="{3FDC604F-37A2-464A-9E1A-14A6423DCD4F}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="207">
   <si>
     <t>email</t>
   </si>
@@ -585,23 +585,89 @@
     <t>Fritch</t>
   </si>
   <si>
-    <t>Sadie</t>
-  </si>
-  <si>
-    <t>Drouin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sadie is a Research Associate I for the McCarroll &amp; Macosko BICAN project. She is a recent graduate from Wheaton College MA with a B.S. in Neuroscience on the Pre-Medical Track. Prior to joining the BICAN project, in her Behavioral Neuroscience lab she completed a senior honors thesis titled: The effects of maternal separation and social isolation on memory and myelin in adolescent rats. In addition to being a research associate, she is also a medical assistant in primary care and sports medicine at DMC primary care. </t>
-  </si>
-  <si>
-    <t>drouin@broadinstitute.org</t>
+    <t>Kathleen is a Research Associate I working on the BICAN project for the McCarroll &amp; Macosko labs and studying X-linked Dystonia Parkinsonism. Prior to joining the Broad, she researched transgenerational epigenetic inheritance and adaptation using C. Elegans at Boston Children’s Hospital and earned a B.A. in Biochemistry from Wellesley College.</t>
+  </si>
+  <si>
+    <t>Kathleen</t>
+  </si>
+  <si>
+    <t>Kim</t>
+  </si>
+  <si>
+    <t>kimkathl@broadinstitute.org</t>
+  </si>
+  <si>
+    <t>Altea</t>
+  </si>
+  <si>
+    <t>Thompson</t>
+  </si>
+  <si>
+    <t>athompso@broadinstitute.org</t>
+  </si>
+  <si>
+    <t>Altea is an undergraduate co-op from Tufts University, studying biotechnology and math. She is a member of the Broad Institute of MIT and Harvard and works in the Stanley Center in the Macosko Lab.</t>
+  </si>
+  <si>
+    <t>Emily</t>
+  </si>
+  <si>
+    <t>Finn</t>
+  </si>
+  <si>
+    <t>Valerie</t>
+  </si>
+  <si>
+    <t>Foley</t>
+  </si>
+  <si>
+    <t>Langlieb</t>
+  </si>
+  <si>
+    <t>Mukund</t>
+  </si>
+  <si>
+    <t>Raj</t>
+  </si>
+  <si>
+    <t>Silverman</t>
+  </si>
+  <si>
+    <t>finnemil@broadinstitute.org</t>
+  </si>
+  <si>
+    <t>foley@broadinstitute.org</t>
+  </si>
+  <si>
+    <t>jlanglie@broadinstitute.org</t>
+  </si>
+  <si>
+    <t>mraj@broadinstitute.org</t>
+  </si>
+  <si>
+    <t>jsilverm@broadinstitute.org</t>
+  </si>
+  <si>
+    <t>Emily is a Project Coordinator for the Center for Human Brain Variation focused on advancing various project components for BICAN. Prior to joining the Broad team, Emily managed multiple projects in the Boston College Cognitive and Affective Neuroscience Laboratory including an examination of emotional memory processes in individuals with Down syndrome. Emily earned her B.S. in Neuroscience at Boston College.</t>
+  </si>
+  <si>
+    <t>Valerie Foley is an undergraduate co-op student working as a Research Assistant on the BICAN project. She is pursuing her B.S. in Behavioral Neuroscience with a minor in Biomedical Engineering. Prior to joining The Broad, Valerie worked at The Affective and Brain Sciences Lab at Northeastern University as a Research Assistant, studying the neural basis of social and emotional intelligence in humans, using fNIRS and fMRI data.</t>
+  </si>
+  <si>
+    <t>Jonah is a Senior Computational Associate in the Macosko Lab. His research focuses on developing and applying methods to analyze large-scale single-cell datasets and is excited to work with all this data! Prior to joining the Broad, he studied computer science and math at Swarthmore college.</t>
+  </si>
+  <si>
+    <t>Jonah is an Associate Computational Biologist in the Macosko Lab. His work focuses on the application and development of computational methods for the processing and analysis of single-cell datasets.</t>
+  </si>
+  <si>
+    <t>Mukund is a Senior Software Engineer in the Macosko Lab. He enjoys building interactive, visual analytic web portals, as well as developing visualizations for large, geometric, or high-dimensional datasets. Previously, he received his PhD in computing from the University of Utah with a focus on visualizations for ensemble data and graphs.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -631,6 +697,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -653,11 +725,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -973,10 +1046,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{913DB89F-B24C-9A40-89FD-2CA7843C4F41}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:H36"/>
+      <selection activeCell="A36" sqref="A36:H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1009,189 +1082,177 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>142</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>143</v>
       </c>
       <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>97</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="F2" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="G2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="H2" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="G3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>127</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="H4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>144</v>
       </c>
       <c r="B5" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="C5">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>97</v>
+        <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="F5" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="H5" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>179</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>180</v>
       </c>
       <c r="C6">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D6" t="s">
         <v>97</v>
       </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>91</v>
+      <c r="F6" t="s">
+        <v>177</v>
       </c>
       <c r="G6" t="s">
-        <v>13</v>
+        <v>178</v>
       </c>
       <c r="H6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>102</v>
+        <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="F7" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G7" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="H7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>179</v>
+        <v>118</v>
       </c>
       <c r="B8" t="s">
-        <v>180</v>
+        <v>119</v>
       </c>
       <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8" t="s">
-        <v>97</v>
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
       </c>
       <c r="F8" t="s">
-        <v>177</v>
+        <v>70</v>
       </c>
       <c r="G8" t="s">
-        <v>178</v>
+        <v>19</v>
       </c>
       <c r="H8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>166</v>
+        <v>104</v>
       </c>
       <c r="B9" t="s">
-        <v>167</v>
+        <v>105</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -1199,37 +1260,37 @@
       <c r="D9" t="s">
         <v>97</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>95</v>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>64</v>
       </c>
       <c r="G9" t="s">
-        <v>96</v>
+        <v>5</v>
       </c>
       <c r="H9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>128</v>
+        <v>166</v>
       </c>
       <c r="B10" t="s">
-        <v>129</v>
+        <v>167</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" t="s">
         <v>97</v>
       </c>
-      <c r="E10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" t="s">
-        <v>75</v>
+      <c r="F10" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="G10" t="s">
-        <v>32</v>
+        <v>96</v>
       </c>
       <c r="H10" t="s">
         <v>28</v>
@@ -1237,81 +1298,100 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="B11" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="C11">
-        <v>5</v>
-      </c>
-      <c r="F11" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" t="s">
+        <v>84</v>
+      </c>
       <c r="G11" t="s">
-        <v>171</v>
+        <v>51</v>
       </c>
       <c r="H11" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B12" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="E12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13" t="s">
         <v>6</v>
       </c>
-      <c r="E12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" t="s">
-        <v>76</v>
-      </c>
-      <c r="G12" t="s">
-        <v>34</v>
-      </c>
-      <c r="H12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C13">
+      <c r="F13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G13" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="F13" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G13" t="s">
-        <v>93</v>
-      </c>
       <c r="H13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>164</v>
+        <v>128</v>
       </c>
       <c r="B14" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="C14">
-        <v>8</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>94</v>
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>97</v>
+      </c>
+      <c r="E14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" t="s">
+        <v>75</v>
       </c>
       <c r="G14" t="s">
-        <v>172</v>
+        <v>32</v>
       </c>
       <c r="H14" t="s">
         <v>28</v>
@@ -1319,48 +1399,40 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="B15" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="C15">
-        <v>9</v>
-      </c>
-      <c r="D15" t="s">
-        <v>97</v>
+        <v>4</v>
       </c>
       <c r="E15" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="F15" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="G15" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="H15" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="B16" t="s">
-        <v>135</v>
+        <v>163</v>
       </c>
       <c r="C16">
-        <v>10</v>
-      </c>
-      <c r="E16" t="s">
-        <v>37</v>
-      </c>
-      <c r="F16" t="s">
-        <v>78</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F16" s="1"/>
       <c r="G16" t="s">
-        <v>38</v>
+        <v>171</v>
       </c>
       <c r="H16" t="s">
         <v>28</v>
@@ -1368,143 +1440,143 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>136</v>
+        <v>108</v>
       </c>
       <c r="B17" t="s">
-        <v>137</v>
+        <v>109</v>
       </c>
       <c r="C17">
-        <v>11</v>
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>101</v>
       </c>
       <c r="E17" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="F17" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="G17" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="H17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>138</v>
+        <v>173</v>
       </c>
       <c r="B18" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="C18">
-        <v>12</v>
-      </c>
-      <c r="D18" t="s">
-        <v>99</v>
-      </c>
-      <c r="E18" t="s">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="F18" t="s">
-        <v>80</v>
+        <v>175</v>
       </c>
       <c r="G18" t="s">
-        <v>42</v>
+        <v>176</v>
       </c>
       <c r="H18" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="B19" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="C19">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="F19" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G19" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="H19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="B20" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>99</v>
       </c>
       <c r="E20" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F20" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="G20" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="H20" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>144</v>
+        <v>110</v>
       </c>
       <c r="B21" t="s">
-        <v>145</v>
+        <v>111</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>97</v>
       </c>
       <c r="E21" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="F21" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="G21" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="H21" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>146</v>
+      <c r="A22" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="B22" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C22">
-        <v>3</v>
-      </c>
-      <c r="D22" t="s">
-        <v>97</v>
+        <v>6</v>
       </c>
       <c r="E22" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F22" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G22" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="H22" t="s">
         <v>45</v>
@@ -1512,137 +1584,138 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="B23" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="C23">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E23" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="F23" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="G23" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="H23" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>173</v>
+        <v>112</v>
       </c>
       <c r="B24" t="s">
-        <v>174</v>
+        <v>113</v>
       </c>
       <c r="C24">
-        <v>5</v>
-      </c>
-      <c r="F24" t="s">
-        <v>175</v>
+        <v>7</v>
+      </c>
+      <c r="D24" t="s">
+        <v>97</v>
+      </c>
+      <c r="E24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="G24" t="s">
-        <v>176</v>
+        <v>13</v>
       </c>
       <c r="H24" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>150</v>
+      <c r="A25" t="s">
+        <v>152</v>
       </c>
       <c r="B25" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C25">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="D25" t="s">
+        <v>100</v>
       </c>
       <c r="E25" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F25" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G25" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H25" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>152</v>
-      </c>
-      <c r="B26" t="s">
-        <v>153</v>
+      <c r="A26" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>161</v>
       </c>
       <c r="C26">
         <v>7</v>
       </c>
-      <c r="D26" t="s">
-        <v>100</v>
-      </c>
-      <c r="E26" t="s">
-        <v>56</v>
-      </c>
-      <c r="F26" t="s">
-        <v>87</v>
+      <c r="D26" s="2"/>
+      <c r="F26" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="G26" t="s">
-        <v>57</v>
+        <v>93</v>
       </c>
       <c r="H26" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="B27" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="C27">
         <v>8</v>
       </c>
-      <c r="E27" t="s">
-        <v>58</v>
-      </c>
-      <c r="F27" t="s">
-        <v>88</v>
+      <c r="F27" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="G27" t="s">
-        <v>59</v>
+        <v>172</v>
       </c>
       <c r="H27" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B28" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C28">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G28" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H28" t="s">
         <v>45</v>
@@ -1650,25 +1723,22 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B29" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C29">
-        <v>10</v>
-      </c>
-      <c r="D29" t="s">
-        <v>97</v>
+        <v>9</v>
       </c>
       <c r="E29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G29" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H29" t="s">
         <v>45</v>
@@ -1676,177 +1746,281 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="B30" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E30" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="F30" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="G30" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="H30" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>116</v>
+        <v>158</v>
       </c>
       <c r="B31" t="s">
-        <v>117</v>
+        <v>159</v>
       </c>
       <c r="C31">
-        <v>2</v>
+        <v>10</v>
+      </c>
+      <c r="D31" t="s">
+        <v>97</v>
       </c>
       <c r="E31" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="F31" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="G31" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="H31" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="B32" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="C32">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E32" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="F32" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="G32" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="H32" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="B33" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C33">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E33" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="F33" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="G33" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="H33" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="B34" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
       <c r="C34">
-        <v>5</v>
+        <v>12</v>
+      </c>
+      <c r="D34" t="s">
+        <v>99</v>
       </c>
       <c r="E34" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="F34" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="G34" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="H34" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="B35" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
       <c r="C35">
-        <v>6</v>
-      </c>
-      <c r="D35" t="s">
-        <v>99</v>
+        <v>13</v>
       </c>
       <c r="E35" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="F35" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="G35" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="H35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="H36" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B41" t="s">
+        <v>186</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="H41" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>182</v>
+      </c>
+      <c r="B42" t="s">
+        <v>183</v>
+      </c>
+      <c r="F42" t="s">
+        <v>184</v>
+      </c>
+      <c r="G42" t="s">
         <v>181</v>
       </c>
-      <c r="B36" t="s">
-        <v>182</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="G36" t="s">
-        <v>183</v>
-      </c>
-      <c r="H36" t="s">
+      <c r="H42" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:H34" xr:uid="{913DB89F-B24C-9A40-89FD-2CA7843C4F41}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H35">
-      <sortCondition ref="H1:H35"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H42">
+      <sortCondition ref="C1:C42"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="F6" r:id="rId1" xr:uid="{EF70C838-9454-A340-875B-3D4829496F9E}"/>
-    <hyperlink ref="F13" r:id="rId2" xr:uid="{5DEF1B66-0C25-744A-8D21-CF21443745D2}"/>
-    <hyperlink ref="F14" r:id="rId3" xr:uid="{05B46BA3-D647-FD42-AB3D-3CEEFA5D5FF1}"/>
-    <hyperlink ref="F9" r:id="rId4" xr:uid="{24BE637A-2716-3B49-A1E8-71436F3E485C}"/>
-    <hyperlink ref="F36" r:id="rId5" xr:uid="{06EDA934-8DE4-0A41-88B2-4E0BE023A029}"/>
+    <hyperlink ref="F24" r:id="rId1" xr:uid="{EF70C838-9454-A340-875B-3D4829496F9E}"/>
+    <hyperlink ref="F26" r:id="rId2" xr:uid="{5DEF1B66-0C25-744A-8D21-CF21443745D2}"/>
+    <hyperlink ref="F27" r:id="rId3" xr:uid="{05B46BA3-D647-FD42-AB3D-3CEEFA5D5FF1}"/>
+    <hyperlink ref="F10" r:id="rId4" xr:uid="{24BE637A-2716-3B49-A1E8-71436F3E485C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1854,10 +2028,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C47BFFC-A8EF-3F42-B9D9-B405CCCF7827}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H2"/>
+      <selection activeCell="A2" sqref="A2:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1889,26 +2063,91 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>181</v>
-      </c>
-      <c r="B2" t="s">
-        <v>182</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="G2" t="s">
-        <v>183</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="A2" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{6760BC2D-FC9E-B14B-A80F-A06DBA6C649E}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Deploying to gh-pages from @ broadinstitute/chbv@65fb8ddb083ffd9d4e951b74760a94df93350015 🚀
</commit_message>
<xml_diff>
--- a/people.xlsx
+++ b/people.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nrockwei/Library/CloudStorage/OneDrive-Personal/sm_lab/projects/websites/chbv/chbv/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c3f52bd1882c5245/sm_lab/projects/websites/chbv/chbv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946DABF0-E1AB-CC46-8D1A-EF3775259AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="219" documentId="8_{EADF6017-5F87-0A4F-AF0D-7723D1C651F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{149D7C51-487F-934C-B96E-F05B3E4FC7A1}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="500" windowWidth="34700" windowHeight="20720" activeTab="1" xr2:uid="{3FDC604F-37A2-464A-9E1A-14A6423DCD4F}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="207">
   <si>
     <t>email</t>
   </si>
@@ -585,23 +585,89 @@
     <t>Fritch</t>
   </si>
   <si>
-    <t>Sadie</t>
-  </si>
-  <si>
-    <t>Drouin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sadie is a Research Associate I for the McCarroll &amp; Macosko BICAN project. She is a recent graduate from Wheaton College MA with a B.S. in Neuroscience on the Pre-Medical Track. Prior to joining the BICAN project, in her Behavioral Neuroscience lab she completed a senior honors thesis titled: The effects of maternal separation and social isolation on memory and myelin in adolescent rats. In addition to being a research associate, she is also a medical assistant in primary care and sports medicine at DMC primary care. </t>
-  </si>
-  <si>
-    <t>drouin@broadinstitute.org</t>
+    <t>Kathleen is a Research Associate I working on the BICAN project for the McCarroll &amp; Macosko labs and studying X-linked Dystonia Parkinsonism. Prior to joining the Broad, she researched transgenerational epigenetic inheritance and adaptation using C. Elegans at Boston Children’s Hospital and earned a B.A. in Biochemistry from Wellesley College.</t>
+  </si>
+  <si>
+    <t>Kathleen</t>
+  </si>
+  <si>
+    <t>Kim</t>
+  </si>
+  <si>
+    <t>kimkathl@broadinstitute.org</t>
+  </si>
+  <si>
+    <t>Altea</t>
+  </si>
+  <si>
+    <t>Thompson</t>
+  </si>
+  <si>
+    <t>athompso@broadinstitute.org</t>
+  </si>
+  <si>
+    <t>Altea is an undergraduate co-op from Tufts University, studying biotechnology and math. She is a member of the Broad Institute of MIT and Harvard and works in the Stanley Center in the Macosko Lab.</t>
+  </si>
+  <si>
+    <t>Emily</t>
+  </si>
+  <si>
+    <t>Finn</t>
+  </si>
+  <si>
+    <t>Valerie</t>
+  </si>
+  <si>
+    <t>Foley</t>
+  </si>
+  <si>
+    <t>Langlieb</t>
+  </si>
+  <si>
+    <t>Mukund</t>
+  </si>
+  <si>
+    <t>Raj</t>
+  </si>
+  <si>
+    <t>Silverman</t>
+  </si>
+  <si>
+    <t>finnemil@broadinstitute.org</t>
+  </si>
+  <si>
+    <t>foley@broadinstitute.org</t>
+  </si>
+  <si>
+    <t>jlanglie@broadinstitute.org</t>
+  </si>
+  <si>
+    <t>mraj@broadinstitute.org</t>
+  </si>
+  <si>
+    <t>jsilverm@broadinstitute.org</t>
+  </si>
+  <si>
+    <t>Emily is a Project Coordinator for the Center for Human Brain Variation focused on advancing various project components for BICAN. Prior to joining the Broad team, Emily managed multiple projects in the Boston College Cognitive and Affective Neuroscience Laboratory including an examination of emotional memory processes in individuals with Down syndrome. Emily earned her B.S. in Neuroscience at Boston College.</t>
+  </si>
+  <si>
+    <t>Valerie Foley is an undergraduate co-op student working as a Research Assistant on the BICAN project. She is pursuing her B.S. in Behavioral Neuroscience with a minor in Biomedical Engineering. Prior to joining The Broad, Valerie worked at The Affective and Brain Sciences Lab at Northeastern University as a Research Assistant, studying the neural basis of social and emotional intelligence in humans, using fNIRS and fMRI data.</t>
+  </si>
+  <si>
+    <t>Jonah is a Senior Computational Associate in the Macosko Lab. His research focuses on developing and applying methods to analyze large-scale single-cell datasets and is excited to work with all this data! Prior to joining the Broad, he studied computer science and math at Swarthmore college.</t>
+  </si>
+  <si>
+    <t>Jonah is an Associate Computational Biologist in the Macosko Lab. His work focuses on the application and development of computational methods for the processing and analysis of single-cell datasets.</t>
+  </si>
+  <si>
+    <t>Mukund is a Senior Software Engineer in the Macosko Lab. He enjoys building interactive, visual analytic web portals, as well as developing visualizations for large, geometric, or high-dimensional datasets. Previously, he received his PhD in computing from the University of Utah with a focus on visualizations for ensemble data and graphs.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -631,6 +697,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -653,11 +725,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -973,10 +1046,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{913DB89F-B24C-9A40-89FD-2CA7843C4F41}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:H36"/>
+      <selection activeCell="A36" sqref="A36:H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1009,189 +1082,177 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>142</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>143</v>
       </c>
       <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>97</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="F2" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="G2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="H2" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="G3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>127</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="H4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>144</v>
       </c>
       <c r="B5" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="C5">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>97</v>
+        <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="F5" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="H5" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>179</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>180</v>
       </c>
       <c r="C6">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D6" t="s">
         <v>97</v>
       </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>91</v>
+      <c r="F6" t="s">
+        <v>177</v>
       </c>
       <c r="G6" t="s">
-        <v>13</v>
+        <v>178</v>
       </c>
       <c r="H6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>102</v>
+        <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="F7" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G7" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="H7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>179</v>
+        <v>118</v>
       </c>
       <c r="B8" t="s">
-        <v>180</v>
+        <v>119</v>
       </c>
       <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8" t="s">
-        <v>97</v>
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
       </c>
       <c r="F8" t="s">
-        <v>177</v>
+        <v>70</v>
       </c>
       <c r="G8" t="s">
-        <v>178</v>
+        <v>19</v>
       </c>
       <c r="H8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>166</v>
+        <v>104</v>
       </c>
       <c r="B9" t="s">
-        <v>167</v>
+        <v>105</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -1199,37 +1260,37 @@
       <c r="D9" t="s">
         <v>97</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>95</v>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>64</v>
       </c>
       <c r="G9" t="s">
-        <v>96</v>
+        <v>5</v>
       </c>
       <c r="H9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>128</v>
+        <v>166</v>
       </c>
       <c r="B10" t="s">
-        <v>129</v>
+        <v>167</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" t="s">
         <v>97</v>
       </c>
-      <c r="E10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" t="s">
-        <v>75</v>
+      <c r="F10" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="G10" t="s">
-        <v>32</v>
+        <v>96</v>
       </c>
       <c r="H10" t="s">
         <v>28</v>
@@ -1237,81 +1298,100 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="B11" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="C11">
-        <v>5</v>
-      </c>
-      <c r="F11" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" t="s">
+        <v>84</v>
+      </c>
       <c r="G11" t="s">
-        <v>171</v>
+        <v>51</v>
       </c>
       <c r="H11" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B12" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="E12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13" t="s">
         <v>6</v>
       </c>
-      <c r="E12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" t="s">
-        <v>76</v>
-      </c>
-      <c r="G12" t="s">
-        <v>34</v>
-      </c>
-      <c r="H12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C13">
+      <c r="F13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G13" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="F13" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G13" t="s">
-        <v>93</v>
-      </c>
       <c r="H13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>164</v>
+        <v>128</v>
       </c>
       <c r="B14" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="C14">
-        <v>8</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>94</v>
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>97</v>
+      </c>
+      <c r="E14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" t="s">
+        <v>75</v>
       </c>
       <c r="G14" t="s">
-        <v>172</v>
+        <v>32</v>
       </c>
       <c r="H14" t="s">
         <v>28</v>
@@ -1319,48 +1399,40 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="B15" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="C15">
-        <v>9</v>
-      </c>
-      <c r="D15" t="s">
-        <v>97</v>
+        <v>4</v>
       </c>
       <c r="E15" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="F15" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="G15" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="H15" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="B16" t="s">
-        <v>135</v>
+        <v>163</v>
       </c>
       <c r="C16">
-        <v>10</v>
-      </c>
-      <c r="E16" t="s">
-        <v>37</v>
-      </c>
-      <c r="F16" t="s">
-        <v>78</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F16" s="1"/>
       <c r="G16" t="s">
-        <v>38</v>
+        <v>171</v>
       </c>
       <c r="H16" t="s">
         <v>28</v>
@@ -1368,143 +1440,143 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>136</v>
+        <v>108</v>
       </c>
       <c r="B17" t="s">
-        <v>137</v>
+        <v>109</v>
       </c>
       <c r="C17">
-        <v>11</v>
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>101</v>
       </c>
       <c r="E17" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="F17" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="G17" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="H17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>138</v>
+        <v>173</v>
       </c>
       <c r="B18" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="C18">
-        <v>12</v>
-      </c>
-      <c r="D18" t="s">
-        <v>99</v>
-      </c>
-      <c r="E18" t="s">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="F18" t="s">
-        <v>80</v>
+        <v>175</v>
       </c>
       <c r="G18" t="s">
-        <v>42</v>
+        <v>176</v>
       </c>
       <c r="H18" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="B19" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="C19">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="F19" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G19" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="H19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="B20" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>99</v>
       </c>
       <c r="E20" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F20" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="G20" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="H20" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>144</v>
+        <v>110</v>
       </c>
       <c r="B21" t="s">
-        <v>145</v>
+        <v>111</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>97</v>
       </c>
       <c r="E21" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="F21" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="G21" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="H21" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>146</v>
+      <c r="A22" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="B22" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C22">
-        <v>3</v>
-      </c>
-      <c r="D22" t="s">
-        <v>97</v>
+        <v>6</v>
       </c>
       <c r="E22" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F22" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G22" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="H22" t="s">
         <v>45</v>
@@ -1512,137 +1584,138 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="B23" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="C23">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E23" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="F23" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="G23" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="H23" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>173</v>
+        <v>112</v>
       </c>
       <c r="B24" t="s">
-        <v>174</v>
+        <v>113</v>
       </c>
       <c r="C24">
-        <v>5</v>
-      </c>
-      <c r="F24" t="s">
-        <v>175</v>
+        <v>7</v>
+      </c>
+      <c r="D24" t="s">
+        <v>97</v>
+      </c>
+      <c r="E24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="G24" t="s">
-        <v>176</v>
+        <v>13</v>
       </c>
       <c r="H24" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>150</v>
+      <c r="A25" t="s">
+        <v>152</v>
       </c>
       <c r="B25" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C25">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="D25" t="s">
+        <v>100</v>
       </c>
       <c r="E25" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F25" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G25" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H25" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>152</v>
-      </c>
-      <c r="B26" t="s">
-        <v>153</v>
+      <c r="A26" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>161</v>
       </c>
       <c r="C26">
         <v>7</v>
       </c>
-      <c r="D26" t="s">
-        <v>100</v>
-      </c>
-      <c r="E26" t="s">
-        <v>56</v>
-      </c>
-      <c r="F26" t="s">
-        <v>87</v>
+      <c r="D26" s="2"/>
+      <c r="F26" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="G26" t="s">
-        <v>57</v>
+        <v>93</v>
       </c>
       <c r="H26" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="B27" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="C27">
         <v>8</v>
       </c>
-      <c r="E27" t="s">
-        <v>58</v>
-      </c>
-      <c r="F27" t="s">
-        <v>88</v>
+      <c r="F27" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="G27" t="s">
-        <v>59</v>
+        <v>172</v>
       </c>
       <c r="H27" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B28" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C28">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G28" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H28" t="s">
         <v>45</v>
@@ -1650,25 +1723,22 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B29" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C29">
-        <v>10</v>
-      </c>
-      <c r="D29" t="s">
-        <v>97</v>
+        <v>9</v>
       </c>
       <c r="E29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G29" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H29" t="s">
         <v>45</v>
@@ -1676,177 +1746,281 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="B30" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E30" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="F30" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="G30" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="H30" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>116</v>
+        <v>158</v>
       </c>
       <c r="B31" t="s">
-        <v>117</v>
+        <v>159</v>
       </c>
       <c r="C31">
-        <v>2</v>
+        <v>10</v>
+      </c>
+      <c r="D31" t="s">
+        <v>97</v>
       </c>
       <c r="E31" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="F31" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="G31" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="H31" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="B32" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="C32">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E32" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="F32" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="G32" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="H32" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="B33" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C33">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E33" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="F33" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="G33" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="H33" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="B34" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
       <c r="C34">
-        <v>5</v>
+        <v>12</v>
+      </c>
+      <c r="D34" t="s">
+        <v>99</v>
       </c>
       <c r="E34" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="F34" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="G34" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="H34" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="B35" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
       <c r="C35">
-        <v>6</v>
-      </c>
-      <c r="D35" t="s">
-        <v>99</v>
+        <v>13</v>
       </c>
       <c r="E35" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="F35" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="G35" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="H35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="H36" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B41" t="s">
+        <v>186</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="H41" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>182</v>
+      </c>
+      <c r="B42" t="s">
+        <v>183</v>
+      </c>
+      <c r="F42" t="s">
+        <v>184</v>
+      </c>
+      <c r="G42" t="s">
         <v>181</v>
       </c>
-      <c r="B36" t="s">
-        <v>182</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="G36" t="s">
-        <v>183</v>
-      </c>
-      <c r="H36" t="s">
+      <c r="H42" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:H34" xr:uid="{913DB89F-B24C-9A40-89FD-2CA7843C4F41}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H35">
-      <sortCondition ref="H1:H35"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H42">
+      <sortCondition ref="C1:C42"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="F6" r:id="rId1" xr:uid="{EF70C838-9454-A340-875B-3D4829496F9E}"/>
-    <hyperlink ref="F13" r:id="rId2" xr:uid="{5DEF1B66-0C25-744A-8D21-CF21443745D2}"/>
-    <hyperlink ref="F14" r:id="rId3" xr:uid="{05B46BA3-D647-FD42-AB3D-3CEEFA5D5FF1}"/>
-    <hyperlink ref="F9" r:id="rId4" xr:uid="{24BE637A-2716-3B49-A1E8-71436F3E485C}"/>
-    <hyperlink ref="F36" r:id="rId5" xr:uid="{06EDA934-8DE4-0A41-88B2-4E0BE023A029}"/>
+    <hyperlink ref="F24" r:id="rId1" xr:uid="{EF70C838-9454-A340-875B-3D4829496F9E}"/>
+    <hyperlink ref="F26" r:id="rId2" xr:uid="{5DEF1B66-0C25-744A-8D21-CF21443745D2}"/>
+    <hyperlink ref="F27" r:id="rId3" xr:uid="{05B46BA3-D647-FD42-AB3D-3CEEFA5D5FF1}"/>
+    <hyperlink ref="F10" r:id="rId4" xr:uid="{24BE637A-2716-3B49-A1E8-71436F3E485C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1854,10 +2028,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C47BFFC-A8EF-3F42-B9D9-B405CCCF7827}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H2"/>
+      <selection activeCell="A2" sqref="A2:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1889,26 +2063,91 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>181</v>
-      </c>
-      <c r="B2" t="s">
-        <v>182</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="G2" t="s">
-        <v>183</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="A2" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{6760BC2D-FC9E-B14B-A80F-A06DBA6C649E}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>